<commit_message>
part of labeled data added
</commit_message>
<xml_diff>
--- a/codebook.xlsx
+++ b/codebook.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mike/Desktop/Master-thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\Master-thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{689CDD42-F841-6745-92F9-2FE4090C9194}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{0453CA55-160D-574D-BF0F-C02CEEB17F7A}"/>
+    <workbookView xWindow="945" yWindow="1560" windowWidth="28035" windowHeight="17445"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="76">
   <si>
     <t xml:space="preserve">bar chart: </t>
   </si>
@@ -124,12 +123,6 @@
   </si>
   <si>
     <t>pie</t>
-  </si>
-  <si>
-    <t>Codebook</t>
-  </si>
-  <si>
-    <t>Strategie: op welke manier kun je de tekst visualiseren o.b.v. Regels volgens het boek visual language?</t>
   </si>
   <si>
     <t>Visuele karakteristieken</t>
@@ -261,11 +254,113 @@
       <t>one of the core organizing principles of the GOP was opposing Obama. </t>
     </r>
   </si>
+  <si>
+    <t>Y is greater in a than B</t>
+  </si>
+  <si>
+    <t>A is a larger Y quantity than B</t>
+  </si>
+  <si>
+    <t>B is bought more often than A</t>
+  </si>
+  <si>
+    <t>As x increases in value Y increases</t>
+  </si>
+  <si>
+    <t>As X increases, Y decreases</t>
+  </si>
+  <si>
+    <t>A line, drawn on the XY plane, descending from A to B along the X axis</t>
+  </si>
+  <si>
+    <t>Male's height is higher than that of females's</t>
+  </si>
+  <si>
+    <t>the average male is taller than the average female</t>
+  </si>
+  <si>
+    <t>twelve yr. Olds are taller than 10 yr olds</t>
+  </si>
+  <si>
+    <t>the graph shows a positive correlation between a child's increases in age and height between the ages of 10 and 12</t>
+  </si>
+  <si>
+    <t>height increases with age. (from about 46 inches at 10 to 55 inches at 12)</t>
+  </si>
+  <si>
+    <t>the more male a person is, the taller he/she is</t>
+  </si>
+  <si>
+    <t>Terms</t>
+  </si>
+  <si>
+    <t>higher</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>greater than, less than</t>
+  </si>
+  <si>
+    <t>rising</t>
+  </si>
+  <si>
+    <t>falling</t>
+  </si>
+  <si>
+    <t>increasing, decreasing</t>
+  </si>
+  <si>
+    <t>bar (discrete comparison)</t>
+  </si>
+  <si>
+    <t>line (trend assessment)</t>
+  </si>
+  <si>
+    <t>Codebook: Bars and Lines: A study of graphic communication</t>
+  </si>
+  <si>
+    <t>Codebook: Visual language</t>
+  </si>
+  <si>
+    <t>Typical responses</t>
+  </si>
+  <si>
+    <t>Examples:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verhouding tussen twee of meer dingen die je kunt  tellen is een bar chart </t>
+  </si>
+  <si>
+    <t>discrete variabelen</t>
+  </si>
+  <si>
+    <t>Continue variabelen</t>
+  </si>
+  <si>
+    <t>metingen</t>
+  </si>
+  <si>
+    <t>tellingen</t>
+  </si>
+  <si>
+    <t>Of 858 respondents, 16 percent always recline, 20 percent usually do, 14 percent recline about half the time, 30 percent do only once in a while, and 20 percent never recline.</t>
+  </si>
+  <si>
+    <t>Sum has to be 100%</t>
+  </si>
+  <si>
+    <t>Only 21 percent of 188 parents thought bringing unruly children on a plane was “very rude,”</t>
+  </si>
+  <si>
+    <t>Mexico beats Ethiopia, 81 percent to 9 percent (10 percent undecided)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -339,10 +434,182 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -352,22 +619,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -385,7 +668,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -423,7 +706,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -529,7 +812,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -678,131 +961,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56884329-A4FC-0948-BBFB-855E83DEE4CC}">
-  <dimension ref="A1:G104"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="H9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="101.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" customWidth="1"/>
-    <col min="4" max="4" width="2.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="119.83203125" customWidth="1"/>
-    <col min="7" max="7" width="204.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="101.625" customWidth="1"/>
+    <col min="3" max="3" width="3.375" customWidth="1"/>
+    <col min="4" max="4" width="2.625" customWidth="1"/>
+    <col min="5" max="5" width="87.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.875" customWidth="1"/>
+    <col min="7" max="7" width="70.5" customWidth="1"/>
+    <col min="8" max="8" width="148.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" ht="16.5" thickBot="1">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="E3" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="E4" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="E5" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="4" t="s">
+      <c r="E6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="E7" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" ht="16.5" thickBot="1">
+      <c r="E8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>1</v>
       </c>
@@ -810,7 +1100,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:8" ht="16.5" thickBot="1">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -818,73 +1108,182 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:8">
       <c r="A12" t="s">
         <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="E12" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>1</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="E13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="E14" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="E15" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="E16" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="12"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="E17" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>1</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="E18" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16.5" thickBot="1">
       <c r="A19" t="s">
         <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="E19" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>1</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="E20" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="H20" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="H21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -892,7 +1291,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -900,12 +1299,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -913,7 +1312,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -921,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -929,7 +1328,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>1</v>
       </c>
@@ -937,7 +1336,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -946,25 +1345,25 @@
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="7"/>
+      <c r="A48" s="5"/>
     </row>
     <row r="49" spans="1:1">
-      <c r="A49" s="7"/>
+      <c r="A49" s="5"/>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="7"/>
+      <c r="A50" s="5"/>
     </row>
     <row r="51" spans="1:1">
-      <c r="A51" s="7"/>
+      <c r="A51" s="5"/>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="7"/>
+      <c r="A52" s="5"/>
     </row>
     <row r="53" spans="1:1">
-      <c r="A53" s="7"/>
+      <c r="A53" s="5"/>
     </row>
     <row r="54" spans="1:1">
-      <c r="A54" s="7"/>
+      <c r="A54" s="5"/>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" s="1"/>
@@ -991,64 +1390,65 @@
       <c r="A69" s="2"/>
     </row>
     <row r="71" spans="1:1">
-      <c r="A71" s="7"/>
+      <c r="A71" s="5"/>
     </row>
     <row r="72" spans="1:1">
-      <c r="A72" s="7"/>
+      <c r="A72" s="5"/>
     </row>
     <row r="73" spans="1:1">
-      <c r="A73" s="7"/>
+      <c r="A73" s="5"/>
     </row>
     <row r="74" spans="1:1">
-      <c r="A74" s="7"/>
+      <c r="A74" s="5"/>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="7"/>
+      <c r="A75" s="5"/>
     </row>
     <row r="76" spans="1:1">
-      <c r="A76" s="7"/>
+      <c r="A76" s="5"/>
     </row>
     <row r="93" spans="1:1">
-      <c r="A93" s="6"/>
+      <c r="A93" s="4"/>
     </row>
     <row r="94" spans="1:1">
-      <c r="A94" s="6"/>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" spans="1:1">
-      <c r="A95" s="6"/>
+      <c r="A95" s="4"/>
     </row>
     <row r="96" spans="1:1">
-      <c r="A96" s="6"/>
+      <c r="A96" s="4"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="6"/>
+      <c r="A97" s="4"/>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="6"/>
+      <c r="A98" s="4"/>
     </row>
     <row r="99" spans="1:1">
-      <c r="A99" s="6"/>
+      <c r="A99" s="4"/>
     </row>
     <row r="100" spans="1:1">
-      <c r="A100" s="6"/>
+      <c r="A100" s="4"/>
     </row>
     <row r="101" spans="1:1">
-      <c r="A101" s="6"/>
+      <c r="A101" s="4"/>
     </row>
     <row r="102" spans="1:1">
-      <c r="A102" s="6"/>
+      <c r="A102" s="4"/>
     </row>
     <row r="103" spans="1:1">
-      <c r="A103" s="6"/>
+      <c r="A103" s="4"/>
     </row>
     <row r="104" spans="1:1">
-      <c r="A104" s="6"/>
+      <c r="A104" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" display="https://www.youtube.com/watch?v=kjLrZ2SDDaU" xr:uid="{B69AF004-3F0A-3045-AC55-6108874EA40D}"/>
-    <hyperlink ref="G6" r:id="rId2" location="fn-8" display="https://fivethirtyeight.com/features/should-travelers-avoid-flying-airlines-that-have-had-crashes-in-the-past/ - fn-8" xr:uid="{D264AB72-1C7E-7941-95D2-0E5E1F90961A}"/>
+    <hyperlink ref="G5" r:id="rId1" display="https://www.youtube.com/watch?v=kjLrZ2SDDaU"/>
+    <hyperlink ref="G8" r:id="rId2" location="fn-8" display="https://fivethirtyeight.com/features/should-travelers-avoid-flying-airlines-that-have-had-crashes-in-the-past/ - fn-8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>